<commit_message>
Temaplte file included master tables
</commit_message>
<xml_diff>
--- a/Templateprj/Uploads/SenderIdSampleFile.xlsx
+++ b/Templateprj/Uploads/SenderIdSampleFile.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\New folder\VI_SmsBusinessSolutionWeb\Templateprj\Uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F81C92-F075-4D07-B331-28641523F992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D76779-5D9D-487A-ADC3-FBBD15F2CD59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sender" sheetId="1" r:id="rId1"/>
+    <sheet name="Status" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>TeleMarketer</t>
   </si>
@@ -52,13 +53,25 @@
   </si>
   <si>
     <t>RequestedDate</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Inactive</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,16 +85,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -89,13 +113,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,8 +419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -439,4 +480,43 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E24119BC-E590-4C22-AE5B-BB2CFCCF4B95}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>